<commit_message>
Added a bunch of tests...I'm tired now, will finish LoadConfig and SendEmail tomorrow
</commit_message>
<xml_diff>
--- a/.templates/Data/Configs/DispatcherConfig.xlsx
+++ b/.templates/Data/Configs/DispatcherConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eyash\Documents\UiPath\LazyFramework\.templates\Data\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFF838A-BDEC-4397-948F-B803B7E72C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC1A05A-9886-495C-87E4-7DF404036EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27360" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27360" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>Credentials_Email</t>
+  </si>
+  <si>
+    <t>IMAP_Port</t>
+  </si>
+  <si>
+    <t>IMAP_Server</t>
+  </si>
+  <si>
+    <t>The port of the IMAP server.</t>
+  </si>
+  <si>
+    <t>The URL of the IMAP server.</t>
   </si>
 </sst>
 </file>
@@ -455,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -580,10 +592,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59017D05-C146-4F94-B0C7-FE1042A65B41}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,6 +671,34 @@
       </c>
       <c r="D5" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>